<commit_message>
Uploaded updated transition-level intensity analysis xlsx spreadsheet
</commit_message>
<xml_diff>
--- a/intensity analysis/Transition_Level_Intensity_Analysis.xlsx
+++ b/intensity analysis/Transition_Level_Intensity_Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dondealban/Dropbox/Image Processing/Philippines/Mindoro/6 intensity analysis/2019.08.17 v3 Manuscript/3 transition level/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dondealban/Dropbox/Image Processing/Philippines/Mindoro/6 intensity analysis/2019.08.25 v4 Manuscript/3 transition level/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EB117F-22DF-A94E-85F8-B079404052E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1E71FA-2D2F-9748-86E4-90C0747CDF8D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{7372C83E-2461-C84E-B742-36ACFD4D60C9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{7372C83E-2461-C84E-B742-36ACFD4D60C9}"/>
   </bookViews>
   <sheets>
     <sheet name="FOR_Loss" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="29">
   <si>
     <t>Interval</t>
   </si>
@@ -119,6 +119,9 @@
   <si>
     <t>Mts Iglit-Baco NP</t>
   </si>
+  <si>
+    <t>Mt Siburan KBA</t>
+  </si>
 </sst>
 </file>
 
@@ -202,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -233,6 +236,7 @@
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,9 +551,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C18C1B5-CED0-C943-8D3D-9DD8E975AB88}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2073,422 +2079,982 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>27</v>
+      <c r="B44" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="5">
-        <v>1765.5</v>
+        <v>16.166666030883789</v>
       </c>
       <c r="E44" s="6">
-        <v>0.48492088913917542</v>
+        <v>0.14060415327548981</v>
       </c>
       <c r="F44" s="4">
-        <v>0.84628039598464966</v>
+        <v>0.75936174392700195</v>
       </c>
       <c r="G44" s="7">
-        <v>3229.847412109375</v>
+        <v>94.444343566894531</v>
       </c>
       <c r="H44" s="8">
-        <v>1464.3475341796875</v>
+        <v>78.277671813964844</v>
       </c>
       <c r="I44" s="4">
         <v>0</v>
       </c>
       <c r="J44" s="4">
-        <v>45.337974548339844</v>
+        <v>82.882331848144531</v>
       </c>
       <c r="K44" s="4">
-        <v>1.5770891904830933</v>
+        <v>0.82707405090332031</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>27</v>
+      <c r="B45" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="5">
-        <v>414.58334350585938</v>
+        <v>19.833333969116211</v>
       </c>
       <c r="E45" s="9">
-        <v>2.9753360748291016</v>
+        <v>0.83228421211242676</v>
       </c>
       <c r="F45" s="4">
-        <v>0.84628039598464966</v>
+        <v>0.75936174392700195</v>
       </c>
       <c r="G45" s="10">
-        <v>84.388214111328125</v>
+        <v>17.921365737915039</v>
       </c>
       <c r="H45" s="11">
-        <v>330.19512939453125</v>
+        <v>1.911967396736145</v>
       </c>
       <c r="I45" s="4">
-        <v>79.645057678222656</v>
+        <v>9.640172004699707</v>
       </c>
       <c r="J45" s="4">
         <v>0</v>
       </c>
       <c r="K45" s="4">
-        <v>1.5770889520645142</v>
+        <v>0.82707411050796509</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>27</v>
+      <c r="B46" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D46" s="5">
-        <v>208.25</v>
-      </c>
-      <c r="E46" s="9">
-        <v>1.7770286798477173</v>
+        <v>0</v>
+      </c>
+      <c r="E46" s="6">
+        <v>0</v>
       </c>
       <c r="F46" s="4">
-        <v>0.84628039598464966</v>
-      </c>
-      <c r="G46" s="10">
-        <v>86.846656799316406</v>
-      </c>
-      <c r="H46" s="11">
-        <v>121.40334320068359</v>
+        <v>0.75936174392700195</v>
+      </c>
+      <c r="G46" s="7">
+        <v>9.5914812088012695</v>
+      </c>
+      <c r="H46" s="8">
+        <v>9.5914812088012695</v>
       </c>
       <c r="I46" s="4">
-        <v>58.296920776367188</v>
+        <v>0</v>
       </c>
       <c r="J46" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K46" s="4">
-        <v>1.5770889520645142</v>
+        <v>0.82707405090332031</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>27</v>
+      <c r="B47" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="5">
+        <v>250.58332824707031</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1.1075506210327148</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.75936174392700195</v>
+      </c>
+      <c r="G47" s="10">
+        <v>163.90737915039062</v>
+      </c>
+      <c r="H47" s="11">
+        <v>86.675941467285156</v>
+      </c>
+      <c r="I47" s="4">
+        <v>34.589668273925781</v>
+      </c>
+      <c r="J47" s="4">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4">
+        <v>0.82707411050796509</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="5">
+        <v>8.3333335816860199E-2</v>
+      </c>
+      <c r="E48" s="6">
+        <v>8.5910648107528687E-2</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0.75936174392700195</v>
+      </c>
+      <c r="G48" s="7">
+        <v>0.8020750880241394</v>
+      </c>
+      <c r="H48" s="8">
+        <v>0.71874171495437622</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0</v>
+      </c>
+      <c r="J48" s="4">
+        <v>89.610282897949219</v>
+      </c>
+      <c r="K48" s="4">
+        <v>0.82707405090332031</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="5">
+        <v>146.89999389648438</v>
+      </c>
+      <c r="E49" s="6">
+        <v>1.143635630607605</v>
+      </c>
+      <c r="F49" s="4">
+        <v>1.2482560873031616</v>
+      </c>
+      <c r="G49" s="7">
+        <v>162.25521850585938</v>
+      </c>
+      <c r="H49" s="8">
+        <v>15.355222702026367</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0</v>
+      </c>
+      <c r="J49" s="4">
+        <v>9.463623046875</v>
+      </c>
+      <c r="K49" s="4">
+        <v>0.46562308073043823</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="E50" s="6">
+        <v>0.27301090955734253</v>
+      </c>
+      <c r="F50" s="4">
+        <v>1.2482560873031616</v>
+      </c>
+      <c r="G50" s="7">
+        <v>17.785886764526367</v>
+      </c>
+      <c r="H50" s="8">
+        <v>14.285886764526367</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0</v>
+      </c>
+      <c r="J50" s="4">
+        <v>80.321479797363281</v>
+      </c>
+      <c r="K50" s="4">
+        <v>0.46562308073043823</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1.6000000238418579</v>
+      </c>
+      <c r="E51" s="6">
+        <v>7.3834791779518127E-2</v>
+      </c>
+      <c r="F51" s="4">
+        <v>1.2482560873031616</v>
+      </c>
+      <c r="G51" s="7">
+        <v>30.679586410522461</v>
+      </c>
+      <c r="H51" s="8">
+        <v>29.079586029052734</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0</v>
+      </c>
+      <c r="J51" s="4">
+        <v>94.784805297851562</v>
+      </c>
+      <c r="K51" s="4">
+        <v>0.46562308073043823</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="5">
+        <v>322.20001220703125</v>
+      </c>
+      <c r="E52" s="9">
+        <v>1.4905625581741333</v>
+      </c>
+      <c r="F52" s="4">
+        <v>1.2482560873031616</v>
+      </c>
+      <c r="G52" s="10">
+        <v>262.3525390625</v>
+      </c>
+      <c r="H52" s="11">
+        <v>59.847461700439453</v>
+      </c>
+      <c r="I52" s="4">
+        <v>18.574630737304688</v>
+      </c>
+      <c r="J52" s="4">
+        <v>0</v>
+      </c>
+      <c r="K52" s="4">
+        <v>0.46562305092811584</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0</v>
+      </c>
+      <c r="E53" s="6">
+        <v>0</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1.2482560873031616</v>
+      </c>
+      <c r="G53" s="7">
+        <v>1.1267722845077515</v>
+      </c>
+      <c r="H53" s="8">
+        <v>1.1267722845077515</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0</v>
+      </c>
+      <c r="J53" s="4">
+        <v>100</v>
+      </c>
+      <c r="K53" s="4">
+        <v>0.46562308073043823</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="5">
+        <v>227.60000610351562</v>
+      </c>
+      <c r="E54" s="6">
+        <v>1.7482141256332397</v>
+      </c>
+      <c r="F54" s="4">
+        <v>3.0477340221405029</v>
+      </c>
+      <c r="G54" s="7">
+        <v>427.2010498046875</v>
+      </c>
+      <c r="H54" s="8">
+        <v>199.60104370117188</v>
+      </c>
+      <c r="I54" s="4">
+        <v>0</v>
+      </c>
+      <c r="J54" s="4">
+        <v>46.722976684570312</v>
+      </c>
+      <c r="K54" s="4">
+        <v>1.0346499681472778</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="5">
+        <v>20.600000381469727</v>
+      </c>
+      <c r="E55" s="6">
+        <v>1.3651424646377563</v>
+      </c>
+      <c r="F55" s="4">
+        <v>3.0477340221405029</v>
+      </c>
+      <c r="G55" s="7">
+        <v>50.555061340332031</v>
+      </c>
+      <c r="H55" s="8">
+        <v>29.955059051513672</v>
+      </c>
+      <c r="I55" s="4">
+        <v>0</v>
+      </c>
+      <c r="J55" s="4">
+        <v>59.252346038818359</v>
+      </c>
+      <c r="K55" s="4">
+        <v>1.0346499681472778</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="5">
+        <v>0.20000000298023224</v>
+      </c>
+      <c r="E56" s="6">
+        <v>2.1253984421491623E-2</v>
+      </c>
+      <c r="F56" s="4">
+        <v>3.0477340221405029</v>
+      </c>
+      <c r="G56" s="7">
+        <v>33.799259185791016</v>
+      </c>
+      <c r="H56" s="8">
+        <v>33.599258422851562</v>
+      </c>
+      <c r="I56" s="4">
+        <v>0</v>
+      </c>
+      <c r="J56" s="4">
+        <v>99.408271789550781</v>
+      </c>
+      <c r="K56" s="4">
+        <v>1.0346499681472778</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="5">
+        <v>962.20001220703125</v>
+      </c>
+      <c r="E57" s="9">
+        <v>3.9803092479705811</v>
+      </c>
+      <c r="F57" s="4">
+        <v>3.0477340221405029</v>
+      </c>
+      <c r="G57" s="10">
+        <v>696.22882080078125</v>
+      </c>
+      <c r="H57" s="11">
+        <v>265.97122192382812</v>
+      </c>
+      <c r="I57" s="4">
+        <v>27.641988754272461</v>
+      </c>
+      <c r="J57" s="4">
+        <v>0</v>
+      </c>
+      <c r="K57" s="4">
+        <v>1.0346498489379883</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="5">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+      <c r="F58" s="4">
+        <v>3.0477340221405029</v>
+      </c>
+      <c r="G58" s="7">
+        <v>1.0067863464355469</v>
+      </c>
+      <c r="H58" s="8">
+        <v>1.0067863464355469</v>
+      </c>
+      <c r="I58" s="4">
+        <v>0</v>
+      </c>
+      <c r="J58" s="4">
+        <v>100</v>
+      </c>
+      <c r="K58" s="4">
+        <v>1.0346499681472778</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="5">
+        <v>0.60000002384185791</v>
+      </c>
+      <c r="E59" s="6">
+        <v>0.85714280605316162</v>
+      </c>
+      <c r="F59" s="4">
+        <v>3.0477340221405029</v>
+      </c>
+      <c r="G59" s="7">
+        <v>2.4090960025787354</v>
+      </c>
+      <c r="H59" s="8">
+        <v>1.8090959787368774</v>
+      </c>
+      <c r="I59" s="4">
+        <v>0</v>
+      </c>
+      <c r="J59" s="4">
+        <v>75.094390869140625</v>
+      </c>
+      <c r="K59" s="4">
+        <v>1.0346499681472778</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="5">
+        <v>1765.5</v>
+      </c>
+      <c r="E60" s="6">
+        <v>0.48492088913917542</v>
+      </c>
+      <c r="F60" s="4">
+        <v>0.84628039598464966</v>
+      </c>
+      <c r="G60" s="7">
+        <v>3229.847412109375</v>
+      </c>
+      <c r="H60" s="8">
+        <v>1464.3475341796875</v>
+      </c>
+      <c r="I60" s="4">
+        <v>0</v>
+      </c>
+      <c r="J60" s="4">
+        <v>45.337974548339844</v>
+      </c>
+      <c r="K60" s="4">
+        <v>1.5770891904830933</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="5">
+        <v>414.58334350585938</v>
+      </c>
+      <c r="E61" s="9">
+        <v>2.9753360748291016</v>
+      </c>
+      <c r="F61" s="4">
+        <v>0.84628039598464966</v>
+      </c>
+      <c r="G61" s="10">
+        <v>84.388214111328125</v>
+      </c>
+      <c r="H61" s="11">
+        <v>330.19512939453125</v>
+      </c>
+      <c r="I61" s="4">
+        <v>79.645057678222656</v>
+      </c>
+      <c r="J61" s="4">
+        <v>0</v>
+      </c>
+      <c r="K61" s="4">
+        <v>1.5770889520645142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="5">
+        <v>208.25</v>
+      </c>
+      <c r="E62" s="9">
+        <v>1.7770286798477173</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0.84628039598464966</v>
+      </c>
+      <c r="G62" s="10">
+        <v>86.846656799316406</v>
+      </c>
+      <c r="H62" s="11">
+        <v>121.40334320068359</v>
+      </c>
+      <c r="I62" s="4">
+        <v>58.296920776367188</v>
+      </c>
+      <c r="J62" s="4">
+        <v>0</v>
+      </c>
+      <c r="K62" s="4">
+        <v>1.5770889520645142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="5">
         <v>2189.833251953125</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E63" s="9">
         <v>1.4480820894241333</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F63" s="4">
         <v>0.84628039598464966</v>
       </c>
-      <c r="G47" s="10">
+      <c r="G63" s="10">
         <v>1176.904052734375</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H63" s="11">
         <v>1012.92919921875</v>
       </c>
-      <c r="I47" s="4">
+      <c r="I63" s="4">
         <v>46.255996704101562</v>
       </c>
-      <c r="J47" s="4">
-        <v>0</v>
-      </c>
-      <c r="K47" s="4">
+      <c r="J63" s="4">
+        <v>0</v>
+      </c>
+      <c r="K63" s="4">
         <v>1.5770889520645142</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D64" s="5">
         <v>2002.5999755859375</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E64" s="6">
         <v>0.54803889989852905</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F64" s="4">
         <v>0.84234142303466797</v>
       </c>
-      <c r="G48" s="7">
+      <c r="G64" s="7">
         <v>3176.93603515625</v>
       </c>
-      <c r="H48" s="8">
+      <c r="H64" s="8">
         <v>1174.3359375</v>
       </c>
-      <c r="I48" s="4">
-        <v>0</v>
-      </c>
-      <c r="J48" s="4">
+      <c r="I64" s="4">
+        <v>0</v>
+      </c>
+      <c r="J64" s="4">
         <v>36.964420318603516</v>
       </c>
-      <c r="K48" s="4">
+      <c r="K64" s="4">
         <v>1.1264244318008423</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D65" s="5">
         <v>50.900001525878906</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E65" s="6">
         <v>0.5353386402130127</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F65" s="4">
         <v>0.84234142303466797</v>
       </c>
-      <c r="G49" s="7">
+      <c r="G65" s="7">
         <v>82.774765014648438</v>
       </c>
-      <c r="H49" s="8">
+      <c r="H65" s="8">
         <v>31.874767303466797</v>
       </c>
-      <c r="I49" s="4">
-        <v>0</v>
-      </c>
-      <c r="J49" s="4">
+      <c r="I65" s="4">
+        <v>0</v>
+      </c>
+      <c r="J65" s="4">
         <v>38.507831573486328</v>
       </c>
-      <c r="K49" s="4">
+      <c r="K65" s="4">
         <v>1.1264244318008423</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D66" s="5">
         <v>15.899999618530273</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E66" s="6">
         <v>0.22009965777397156</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F66" s="4">
         <v>0.84234142303466797</v>
       </c>
-      <c r="G50" s="7">
+      <c r="G66" s="7">
         <v>64.98541259765625</v>
       </c>
-      <c r="H50" s="8">
+      <c r="H66" s="8">
         <v>49.085411071777344</v>
       </c>
-      <c r="I50" s="4">
-        <v>0</v>
-      </c>
-      <c r="J50" s="4">
+      <c r="I66" s="4">
+        <v>0</v>
+      </c>
+      <c r="J66" s="4">
         <v>75.532974243164062</v>
       </c>
-      <c r="K50" s="4">
+      <c r="K66" s="4">
         <v>1.1264244318008423</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D67" s="5">
         <v>2365.300048828125</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E67" s="9">
         <v>1.6388365030288696</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F67" s="4">
         <v>0.84234142303466797</v>
       </c>
-      <c r="G51" s="10">
+      <c r="G67" s="10">
         <v>1109.9951171875</v>
       </c>
-      <c r="H51" s="11">
+      <c r="H67" s="11">
         <v>1255.304931640625</v>
       </c>
-      <c r="I51" s="4">
+      <c r="I67" s="4">
         <v>53.071701049804688</v>
       </c>
-      <c r="J51" s="4">
-        <v>0</v>
-      </c>
-      <c r="K51" s="4">
+      <c r="J67" s="4">
+        <v>0</v>
+      </c>
+      <c r="K67" s="4">
         <v>1.1264240741729736</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D68" s="5">
         <v>8712.7998046875</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E68" s="6">
         <v>2.2359433174133301</v>
       </c>
-      <c r="F52" s="4">
+      <c r="F68" s="4">
         <v>3.2488365173339844</v>
       </c>
-      <c r="G52" s="7">
+      <c r="G68" s="7">
         <v>13425.23828125</v>
       </c>
-      <c r="H52" s="8">
+      <c r="H68" s="8">
         <v>4712.43798828125</v>
       </c>
-      <c r="I52" s="4">
-        <v>0</v>
-      </c>
-      <c r="J52" s="4">
+      <c r="I68" s="4">
+        <v>0</v>
+      </c>
+      <c r="J68" s="4">
         <v>35.101337432861328</v>
       </c>
-      <c r="K52" s="4">
+      <c r="K68" s="4">
         <v>2.2027969360351562</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B69" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D69" s="5">
         <v>328.60000610351562</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E69" s="6">
         <v>2.956099271774292</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F69" s="4">
         <v>3.2488365173339844</v>
       </c>
-      <c r="G53" s="7">
+      <c r="G69" s="7">
         <v>367.45184326171875</v>
       </c>
-      <c r="H53" s="8">
+      <c r="H69" s="8">
         <v>38.851833343505859</v>
       </c>
-      <c r="I53" s="4">
-        <v>0</v>
-      </c>
-      <c r="J53" s="4">
+      <c r="I69" s="4">
+        <v>0</v>
+      </c>
+      <c r="J69" s="4">
         <v>10.57331371307373</v>
       </c>
-      <c r="K53" s="4">
+      <c r="K69" s="4">
         <v>2.2027969360351562</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D70" s="5">
         <v>61.599998474121094</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E70" s="6">
         <v>1.0372116565704346</v>
       </c>
-      <c r="F54" s="4">
+      <c r="F70" s="4">
         <v>3.2488365173339844</v>
       </c>
-      <c r="G54" s="7">
+      <c r="G70" s="7">
         <v>218.42301940917969</v>
       </c>
-      <c r="H54" s="8">
+      <c r="H70" s="8">
         <v>156.82302856445312</v>
       </c>
-      <c r="I54" s="4">
-        <v>0</v>
-      </c>
-      <c r="J54" s="4">
+      <c r="I70" s="4">
+        <v>0</v>
+      </c>
+      <c r="J70" s="4">
         <v>71.797843933105469</v>
       </c>
-      <c r="K54" s="4">
+      <c r="K70" s="4">
         <v>2.2027969360351562</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D71" s="5">
         <v>10288.2001953125</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E71" s="9">
         <v>5.4119653701782227</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F71" s="4">
         <v>3.2488365173339844</v>
       </c>
-      <c r="G55" s="10">
+      <c r="G71" s="10">
         <v>5378.53564453125</v>
       </c>
-      <c r="H55" s="11">
+      <c r="H71" s="11">
         <v>4909.66455078125</v>
       </c>
-      <c r="I55" s="4">
+      <c r="I71" s="4">
         <v>47.721317291259766</v>
       </c>
-      <c r="J55" s="4">
-        <v>0</v>
-      </c>
-      <c r="K55" s="4">
+      <c r="J71" s="4">
+        <v>0</v>
+      </c>
+      <c r="K71" s="4">
         <v>2.2027969360351562</v>
       </c>
     </row>
@@ -2499,7 +3065,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678ADD05-A299-AB46-B4EE-7316C7D0F3D0}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
@@ -4025,422 +4591,982 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>27</v>
+      <c r="B44" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="10">
-        <v>2519.666748046875</v>
-      </c>
-      <c r="E44" s="6">
-        <v>0.6353873610496521</v>
+        <v>223.91667175292969</v>
+      </c>
+      <c r="E44" s="9">
+        <v>1.5671658515930176</v>
       </c>
       <c r="F44" s="4">
-        <v>0.66176050901412964</v>
-      </c>
-      <c r="G44" s="7">
-        <v>2633.2724609375</v>
-      </c>
-      <c r="H44" s="8">
-        <v>113.60588836669922</v>
+        <v>0.94604486227035522</v>
+      </c>
+      <c r="G44" s="10">
+        <v>123.80577850341797</v>
+      </c>
+      <c r="H44" s="11">
+        <v>100.11089324951172</v>
       </c>
       <c r="I44" s="4">
-        <v>0</v>
+        <v>44.708995819091797</v>
       </c>
       <c r="J44" s="4">
-        <v>4.3142471313476562</v>
+        <v>0</v>
       </c>
       <c r="K44" s="4">
-        <v>0.18553510308265686</v>
+        <v>0.95221036672592163</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>27</v>
+      <c r="B45" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="10">
-        <v>4</v>
+        <v>1.3333333730697632</v>
       </c>
       <c r="E45" s="6">
-        <v>0.31520882248878479</v>
+        <v>0.35842296481132507</v>
       </c>
       <c r="F45" s="4">
-        <v>0.66176050901412964</v>
+        <v>0.94604486227035522</v>
       </c>
       <c r="G45" s="7">
-        <v>8.7770957946777344</v>
+        <v>3.7992284297943115</v>
       </c>
       <c r="H45" s="8">
-        <v>4.7770962715148926</v>
+        <v>2.4658951759338379</v>
       </c>
       <c r="I45" s="4">
         <v>0</v>
       </c>
       <c r="J45" s="4">
-        <v>54.426841735839844</v>
+        <v>64.905158996582031</v>
       </c>
       <c r="K45" s="4">
-        <v>0.18553510308265686</v>
+        <v>0.95221042633056641</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>27</v>
+      <c r="B46" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D46" s="10">
-        <v>1</v>
+        <v>0.4166666567325592</v>
       </c>
       <c r="E46" s="6">
-        <v>1.3603591360151768E-2</v>
+        <v>2.1860791370272636E-2</v>
       </c>
       <c r="F46" s="4">
-        <v>0.66176050901412964</v>
+        <v>0.94604486227035522</v>
       </c>
       <c r="G46" s="7">
-        <v>52.756027221679688</v>
+        <v>20.287454605102539</v>
       </c>
       <c r="H46" s="8">
-        <v>51.756027221679688</v>
+        <v>19.870786666870117</v>
       </c>
       <c r="I46" s="4">
         <v>0</v>
       </c>
       <c r="J46" s="4">
-        <v>98.104484558105469</v>
+        <v>97.946182250976562</v>
       </c>
       <c r="K46" s="4">
-        <v>0.18553510308265686</v>
+        <v>0.95221042633056641</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>27</v>
+      <c r="B47" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="10">
-        <v>967.66668701171875</v>
-      </c>
-      <c r="E47" s="9">
-        <v>0.7904093861579895</v>
+        <v>136.66667175292969</v>
+      </c>
+      <c r="E47" s="6">
+        <v>0.62765991687774658</v>
       </c>
       <c r="F47" s="4">
-        <v>0.66176050901412964</v>
-      </c>
-      <c r="G47" s="10">
-        <v>796.58087158203125</v>
-      </c>
-      <c r="H47" s="11">
-        <v>171.0858154296875</v>
+        <v>0.94604486227035522</v>
+      </c>
+      <c r="G47" s="7">
+        <v>214.86985778808594</v>
+      </c>
+      <c r="H47" s="8">
+        <v>78.20318603515625</v>
       </c>
       <c r="I47" s="4">
-        <v>17.680242538452148</v>
+        <v>0</v>
       </c>
       <c r="J47" s="4">
-        <v>0</v>
+        <v>36.395606994628906</v>
       </c>
       <c r="K47" s="4">
-        <v>0.18553487956523895</v>
+        <v>0.95221042633056641</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>27</v>
+      <c r="A48" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D48" s="10">
-        <v>2897.800048828125</v>
+        <v>0</v>
       </c>
       <c r="E48" s="6">
-        <v>0.79592400789260864</v>
+        <v>0</v>
       </c>
       <c r="F48" s="4">
-        <v>1.0879968404769897</v>
+        <v>0.94604486227035522</v>
       </c>
       <c r="G48" s="7">
-        <v>4090.998291015625</v>
+        <v>1.4513907432556152</v>
       </c>
       <c r="H48" s="8">
-        <v>1193.1983642578125</v>
+        <v>1.4513907432556152</v>
       </c>
       <c r="I48" s="4">
         <v>0</v>
       </c>
       <c r="J48" s="4">
-        <v>29.166433334350586</v>
+        <v>100</v>
       </c>
       <c r="K48" s="4">
-        <v>1.070810079574585</v>
+        <v>0.95221042633056641</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>27</v>
+      <c r="A49" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D49" s="10">
-        <v>340.5</v>
+        <v>3.8333332538604736</v>
       </c>
       <c r="E49" s="9">
-        <v>2.4436631202697754</v>
+        <v>1.6739445924758911</v>
       </c>
       <c r="F49" s="4">
-        <v>1.0879968404769897</v>
+        <v>0.94604486227035522</v>
       </c>
       <c r="G49" s="10">
-        <v>128.54031372070312</v>
+        <v>1.9529744386672974</v>
       </c>
       <c r="H49" s="11">
-        <v>211.95968627929688</v>
+        <v>1.8803588151931763</v>
       </c>
       <c r="I49" s="4">
-        <v>62.249542236328125</v>
+        <v>49.052841186523438</v>
       </c>
       <c r="J49" s="4">
         <v>0</v>
       </c>
       <c r="K49" s="4">
-        <v>1.0708106756210327</v>
+        <v>0.95221036672592163</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>27</v>
+      <c r="B50" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D50" s="10">
-        <v>148.19999694824219</v>
-      </c>
-      <c r="E50" s="9">
-        <v>1.2646130323410034</v>
+        <v>28.600000381469727</v>
+      </c>
+      <c r="E50" s="6">
+        <v>0.24873891472816467</v>
       </c>
       <c r="F50" s="4">
-        <v>1.0879968404769897</v>
-      </c>
-      <c r="G50" s="10">
-        <v>124.97553253173828</v>
-      </c>
-      <c r="H50" s="11">
-        <v>23.224466323852539</v>
+        <v>1.1930810213088989</v>
+      </c>
+      <c r="G50" s="7">
+        <v>151.88993835449219</v>
+      </c>
+      <c r="H50" s="8">
+        <v>123.28993988037109</v>
       </c>
       <c r="I50" s="4">
-        <v>15.671030044555664</v>
+        <v>0</v>
       </c>
       <c r="J50" s="4">
-        <v>0</v>
+        <v>81.170578002929688</v>
       </c>
       <c r="K50" s="4">
-        <v>1.0708106756210327</v>
+        <v>1.210856556892395</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>27</v>
+      <c r="B51" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D51" s="10">
-        <v>2499.199951171875</v>
-      </c>
-      <c r="E51" s="9">
-        <v>1.6526587009429932</v>
+        <v>14</v>
+      </c>
+      <c r="E51" s="6">
+        <v>0.58749473094940186</v>
       </c>
       <c r="F51" s="4">
-        <v>1.0879968404769897</v>
-      </c>
-      <c r="G51" s="10">
-        <v>1541.0555419921875</v>
-      </c>
-      <c r="H51" s="11">
-        <v>958.1444091796875</v>
+        <v>1.1930810213088989</v>
+      </c>
+      <c r="G51" s="7">
+        <v>30.386117935180664</v>
+      </c>
+      <c r="H51" s="8">
+        <v>16.386117935180664</v>
       </c>
       <c r="I51" s="4">
-        <v>38.338047027587891</v>
+        <v>0</v>
       </c>
       <c r="J51" s="4">
-        <v>0</v>
+        <v>53.926326751708984</v>
       </c>
       <c r="K51" s="4">
-        <v>1.0708106756210327</v>
+        <v>1.210856556892395</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D52" s="10">
-        <v>1876.800048828125</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="E52" s="6">
-        <v>0.51361203193664551</v>
+        <v>8.7108016014099121E-3</v>
       </c>
       <c r="F52" s="4">
-        <v>1.0090925693511963</v>
+        <v>1.1930810213088989</v>
       </c>
       <c r="G52" s="7">
-        <v>3783.549560546875</v>
+        <v>15.538510322570801</v>
       </c>
       <c r="H52" s="8">
-        <v>1906.7496337890625</v>
+        <v>15.438509941101074</v>
       </c>
       <c r="I52" s="4">
         <v>0</v>
       </c>
       <c r="J52" s="4">
-        <v>50.395786285400391</v>
+        <v>99.356437683105469</v>
       </c>
       <c r="K52" s="4">
-        <v>0.88462328910827637</v>
+        <v>1.210856556892395</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D53" s="10">
-        <v>80.199996948242188</v>
-      </c>
-      <c r="E53" s="6">
-        <v>0.84350025653839111</v>
+        <v>407</v>
+      </c>
+      <c r="E53" s="9">
+        <v>1.7988951206207275</v>
       </c>
       <c r="F53" s="4">
-        <v>1.0090925693511963</v>
-      </c>
-      <c r="G53" s="7">
-        <v>96.781112670898438</v>
-      </c>
-      <c r="H53" s="8">
-        <v>16.581111907958984</v>
+        <v>1.1930810213088989</v>
+      </c>
+      <c r="G53" s="10">
+        <v>251.36618041992188</v>
+      </c>
+      <c r="H53" s="11">
+        <v>155.63381958007812</v>
       </c>
       <c r="I53" s="4">
-        <v>0</v>
+        <v>38.239265441894531</v>
       </c>
       <c r="J53" s="4">
-        <v>17.132589340209961</v>
+        <v>0</v>
       </c>
       <c r="K53" s="4">
-        <v>0.88462328910827637</v>
+        <v>1.210856556892395</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D54" s="10">
-        <v>27</v>
+        <v>0.69999998807907104</v>
       </c>
       <c r="E54" s="6">
-        <v>0.37375414371490479</v>
+        <v>0.72164952754974365</v>
       </c>
       <c r="F54" s="4">
-        <v>1.0090925693511963</v>
+        <v>1.1930810213088989</v>
       </c>
       <c r="G54" s="7">
-        <v>75.335601806640625</v>
+        <v>1.2192378044128418</v>
       </c>
       <c r="H54" s="8">
-        <v>48.335601806640625</v>
+        <v>0.51923787593841553</v>
       </c>
       <c r="I54" s="4">
         <v>0</v>
       </c>
       <c r="J54" s="4">
-        <v>64.160369873046875</v>
+        <v>42.587085723876953</v>
       </c>
       <c r="K54" s="4">
-        <v>0.88462328910827637</v>
+        <v>1.210856556892395</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="10">
+        <v>141</v>
+      </c>
+      <c r="E55" s="6">
+        <v>1.0977033376693726</v>
+      </c>
+      <c r="F55" s="4">
+        <v>2.2659192085266113</v>
+      </c>
+      <c r="G55" s="7">
+        <v>310.23046875</v>
+      </c>
+      <c r="H55" s="8">
+        <v>169.23045349121094</v>
+      </c>
+      <c r="I55" s="4">
+        <v>0</v>
+      </c>
+      <c r="J55" s="4">
+        <v>54.549915313720703</v>
+      </c>
+      <c r="K55" s="4">
+        <v>0.9765695333480835</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="10">
+        <v>4.8000001907348633</v>
+      </c>
+      <c r="E56" s="6">
+        <v>0.37441498041152954</v>
+      </c>
+      <c r="F56" s="4">
+        <v>2.2659192085266113</v>
+      </c>
+      <c r="G56" s="7">
+        <v>32.147438049316406</v>
+      </c>
+      <c r="H56" s="8">
+        <v>27.347438812255859</v>
+      </c>
+      <c r="I56" s="4">
+        <v>0</v>
+      </c>
+      <c r="J56" s="4">
+        <v>85.068794250488281</v>
+      </c>
+      <c r="K56" s="4">
+        <v>0.9765695333480835</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="10">
+        <v>2.4000000953674316</v>
+      </c>
+      <c r="E57" s="6">
+        <v>0.11075218766927719</v>
+      </c>
+      <c r="F57" s="4">
+        <v>2.2659192085266113</v>
+      </c>
+      <c r="G57" s="7">
+        <v>55.069740295410156</v>
+      </c>
+      <c r="H57" s="8">
+        <v>52.66973876953125</v>
+      </c>
+      <c r="I57" s="4">
+        <v>0</v>
+      </c>
+      <c r="J57" s="4">
+        <v>95.641891479492188</v>
+      </c>
+      <c r="K57" s="4">
+        <v>0.9765695333480835</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="10">
+        <v>712.4000244140625</v>
+      </c>
+      <c r="E58" s="9">
+        <v>3.2957069873809814</v>
+      </c>
+      <c r="F58" s="4">
+        <v>2.2659192085266113</v>
+      </c>
+      <c r="G58" s="10">
+        <v>461.35919189453125</v>
+      </c>
+      <c r="H58" s="11">
+        <v>251.04084777832031</v>
+      </c>
+      <c r="I58" s="4">
+        <v>35.238750457763672</v>
+      </c>
+      <c r="J58" s="4">
+        <v>0</v>
+      </c>
+      <c r="K58" s="4">
+        <v>0.97656941413879395</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="10">
+        <v>0.20000000298023224</v>
+      </c>
+      <c r="E59" s="6">
+        <v>0.25316455960273743</v>
+      </c>
+      <c r="F59" s="4">
+        <v>2.2659192085266113</v>
+      </c>
+      <c r="G59" s="7">
+        <v>1.9932434558868408</v>
+      </c>
+      <c r="H59" s="8">
+        <v>1.793243408203125</v>
+      </c>
+      <c r="I59" s="4">
+        <v>0</v>
+      </c>
+      <c r="J59" s="4">
+        <v>89.966102600097656</v>
+      </c>
+      <c r="K59" s="4">
+        <v>0.9765695333480835</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C60" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="10">
+        <v>2519.666748046875</v>
+      </c>
+      <c r="E60" s="6">
+        <v>0.6353873610496521</v>
+      </c>
+      <c r="F60" s="4">
+        <v>0.66176050901412964</v>
+      </c>
+      <c r="G60" s="7">
+        <v>2633.2724609375</v>
+      </c>
+      <c r="H60" s="8">
+        <v>113.60588836669922</v>
+      </c>
+      <c r="I60" s="4">
+        <v>0</v>
+      </c>
+      <c r="J60" s="4">
+        <v>4.3142471313476562</v>
+      </c>
+      <c r="K60" s="4">
+        <v>0.18553510308265686</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="10">
+        <v>4</v>
+      </c>
+      <c r="E61" s="6">
+        <v>0.31520882248878479</v>
+      </c>
+      <c r="F61" s="4">
+        <v>0.66176050901412964</v>
+      </c>
+      <c r="G61" s="7">
+        <v>8.7770957946777344</v>
+      </c>
+      <c r="H61" s="8">
+        <v>4.7770962715148926</v>
+      </c>
+      <c r="I61" s="4">
+        <v>0</v>
+      </c>
+      <c r="J61" s="4">
+        <v>54.426841735839844</v>
+      </c>
+      <c r="K61" s="4">
+        <v>0.18553510308265686</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="10">
+        <v>1</v>
+      </c>
+      <c r="E62" s="6">
+        <v>1.3603591360151768E-2</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0.66176050901412964</v>
+      </c>
+      <c r="G62" s="7">
+        <v>52.756027221679688</v>
+      </c>
+      <c r="H62" s="8">
+        <v>51.756027221679688</v>
+      </c>
+      <c r="I62" s="4">
+        <v>0</v>
+      </c>
+      <c r="J62" s="4">
+        <v>98.104484558105469</v>
+      </c>
+      <c r="K62" s="4">
+        <v>0.18553510308265686</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D63" s="10">
+        <v>967.66668701171875</v>
+      </c>
+      <c r="E63" s="9">
+        <v>0.7904093861579895</v>
+      </c>
+      <c r="F63" s="4">
+        <v>0.66176050901412964</v>
+      </c>
+      <c r="G63" s="10">
+        <v>796.58087158203125</v>
+      </c>
+      <c r="H63" s="11">
+        <v>171.0858154296875</v>
+      </c>
+      <c r="I63" s="4">
+        <v>17.680242538452148</v>
+      </c>
+      <c r="J63" s="4">
+        <v>0</v>
+      </c>
+      <c r="K63" s="4">
+        <v>0.18553487956523895</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="10">
+        <v>2897.800048828125</v>
+      </c>
+      <c r="E64" s="6">
+        <v>0.79592400789260864</v>
+      </c>
+      <c r="F64" s="4">
+        <v>1.0879968404769897</v>
+      </c>
+      <c r="G64" s="7">
+        <v>4090.998291015625</v>
+      </c>
+      <c r="H64" s="8">
+        <v>1193.1983642578125</v>
+      </c>
+      <c r="I64" s="4">
+        <v>0</v>
+      </c>
+      <c r="J64" s="4">
+        <v>29.166433334350586</v>
+      </c>
+      <c r="K64" s="4">
+        <v>1.070810079574585</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="10">
+        <v>340.5</v>
+      </c>
+      <c r="E65" s="9">
+        <v>2.4436631202697754</v>
+      </c>
+      <c r="F65" s="4">
+        <v>1.0879968404769897</v>
+      </c>
+      <c r="G65" s="10">
+        <v>128.54031372070312</v>
+      </c>
+      <c r="H65" s="11">
+        <v>211.95968627929688</v>
+      </c>
+      <c r="I65" s="4">
+        <v>62.249542236328125</v>
+      </c>
+      <c r="J65" s="4">
+        <v>0</v>
+      </c>
+      <c r="K65" s="4">
+        <v>1.0708106756210327</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" s="10">
+        <v>148.19999694824219</v>
+      </c>
+      <c r="E66" s="9">
+        <v>1.2646130323410034</v>
+      </c>
+      <c r="F66" s="4">
+        <v>1.0879968404769897</v>
+      </c>
+      <c r="G66" s="10">
+        <v>124.97553253173828</v>
+      </c>
+      <c r="H66" s="11">
+        <v>23.224466323852539</v>
+      </c>
+      <c r="I66" s="4">
+        <v>15.671030044555664</v>
+      </c>
+      <c r="J66" s="4">
+        <v>0</v>
+      </c>
+      <c r="K66" s="4">
+        <v>1.0708106756210327</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="10">
+        <v>2499.199951171875</v>
+      </c>
+      <c r="E67" s="9">
+        <v>1.6526587009429932</v>
+      </c>
+      <c r="F67" s="4">
+        <v>1.0879968404769897</v>
+      </c>
+      <c r="G67" s="10">
+        <v>1541.0555419921875</v>
+      </c>
+      <c r="H67" s="11">
+        <v>958.1444091796875</v>
+      </c>
+      <c r="I67" s="4">
+        <v>38.338047027587891</v>
+      </c>
+      <c r="J67" s="4">
+        <v>0</v>
+      </c>
+      <c r="K67" s="4">
+        <v>1.0708106756210327</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="10">
+        <v>1876.800048828125</v>
+      </c>
+      <c r="E68" s="6">
+        <v>0.51361203193664551</v>
+      </c>
+      <c r="F68" s="4">
+        <v>1.0090925693511963</v>
+      </c>
+      <c r="G68" s="7">
+        <v>3783.549560546875</v>
+      </c>
+      <c r="H68" s="8">
+        <v>1906.7496337890625</v>
+      </c>
+      <c r="I68" s="4">
+        <v>0</v>
+      </c>
+      <c r="J68" s="4">
+        <v>50.395786285400391</v>
+      </c>
+      <c r="K68" s="4">
+        <v>0.88462328910827637</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="10">
+        <v>80.199996948242188</v>
+      </c>
+      <c r="E69" s="6">
+        <v>0.84350025653839111</v>
+      </c>
+      <c r="F69" s="4">
+        <v>1.0090925693511963</v>
+      </c>
+      <c r="G69" s="7">
+        <v>96.781112670898438</v>
+      </c>
+      <c r="H69" s="8">
+        <v>16.581111907958984</v>
+      </c>
+      <c r="I69" s="4">
+        <v>0</v>
+      </c>
+      <c r="J69" s="4">
+        <v>17.132589340209961</v>
+      </c>
+      <c r="K69" s="4">
+        <v>0.88462328910827637</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" s="10">
+        <v>27</v>
+      </c>
+      <c r="E70" s="6">
+        <v>0.37375414371490479</v>
+      </c>
+      <c r="F70" s="4">
+        <v>1.0090925693511963</v>
+      </c>
+      <c r="G70" s="7">
+        <v>75.335601806640625</v>
+      </c>
+      <c r="H70" s="8">
+        <v>48.335601806640625</v>
+      </c>
+      <c r="I70" s="4">
+        <v>0</v>
+      </c>
+      <c r="J70" s="4">
+        <v>64.160369873046875</v>
+      </c>
+      <c r="K70" s="4">
+        <v>0.88462328910827637</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="10">
         <v>3328.60009765625</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E71" s="9">
         <v>2.3062746524810791</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F71" s="4">
         <v>1.0090925693511963</v>
       </c>
-      <c r="G55" s="10">
+      <c r="G71" s="10">
         <v>1356.9229736328125</v>
       </c>
-      <c r="H55" s="11">
+      <c r="H71" s="11">
         <v>1971.6771240234375</v>
       </c>
-      <c r="I55" s="4">
+      <c r="I71" s="4">
         <v>59.234428405761719</v>
       </c>
-      <c r="J55" s="4">
-        <v>0</v>
-      </c>
-      <c r="K55" s="4">
+      <c r="J71" s="4">
+        <v>0</v>
+      </c>
+      <c r="K71" s="4">
         <v>0.88462346792221069</v>
       </c>
     </row>
@@ -4451,7 +5577,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87735636-EAF6-D14E-9970-2F394496BBB4}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
@@ -5977,422 +7103,982 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>27</v>
+      <c r="B44" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D44" s="5">
-        <v>2519.666748046875</v>
-      </c>
-      <c r="E44" s="6">
-        <v>0.43940189480781555</v>
+        <v>223.91667175292969</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0.24665586650371552</v>
       </c>
       <c r="F44" s="4">
-        <v>0.64173471927642822</v>
-      </c>
-      <c r="G44" s="7">
-        <v>3776.708251953125</v>
-      </c>
-      <c r="H44" s="8">
-        <v>1257.0416259765625</v>
+        <v>0.22165922820568085</v>
+      </c>
+      <c r="G44" s="10">
+        <v>200.60438537597656</v>
+      </c>
+      <c r="H44" s="11">
+        <v>23.312284469604492</v>
       </c>
       <c r="I44" s="4">
-        <v>0</v>
+        <v>10.411142349243164</v>
       </c>
       <c r="J44" s="4">
-        <v>33.284053802490234</v>
+        <v>0</v>
       </c>
       <c r="K44" s="4">
-        <v>1.3537958860397339</v>
+        <v>0.21764805912971497</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>27</v>
+      <c r="B45" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="5">
-        <v>221.41667175292969</v>
-      </c>
-      <c r="E45" s="9">
-        <v>1.5890388488769531</v>
+        <v>1.8333333730697632</v>
+      </c>
+      <c r="E45" s="6">
+        <v>7.6933838427066803E-2</v>
       </c>
       <c r="F45" s="4">
-        <v>0.64173471927642822</v>
-      </c>
-      <c r="G45" s="10">
-        <v>78.406356811523438</v>
-      </c>
-      <c r="H45" s="11">
-        <v>143.01031494140625</v>
+        <v>0.22165922820568085</v>
+      </c>
+      <c r="G45" s="7">
+        <v>5.3763813972473145</v>
+      </c>
+      <c r="H45" s="8">
+        <v>3.5430479049682617</v>
       </c>
       <c r="I45" s="4">
-        <v>64.588775634765625</v>
+        <v>0</v>
       </c>
       <c r="J45" s="4">
-        <v>0</v>
+        <v>65.900238037109375</v>
       </c>
       <c r="K45" s="4">
-        <v>1.3537960052490234</v>
+        <v>0.21764804422855377</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>27</v>
+      <c r="B46" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D46" s="5">
-        <v>127.75</v>
-      </c>
-      <c r="E46" s="9">
-        <v>1.0901100635528564</v>
+        <v>0</v>
+      </c>
+      <c r="E46" s="6">
+        <v>0</v>
       </c>
       <c r="F46" s="4">
-        <v>0.64173471927642822</v>
-      </c>
-      <c r="G46" s="10">
-        <v>70.820884704589844</v>
-      </c>
-      <c r="H46" s="11">
-        <v>56.929111480712891</v>
+        <v>0.22165922820568085</v>
+      </c>
+      <c r="G46" s="7">
+        <v>2.6141829490661621</v>
+      </c>
+      <c r="H46" s="8">
+        <v>2.6141829490661621</v>
       </c>
       <c r="I46" s="4">
-        <v>44.562904357910156</v>
+        <v>0</v>
       </c>
       <c r="J46" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K46" s="4">
-        <v>1.3537960052490234</v>
+        <v>0.21764804422855377</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>27</v>
+      <c r="B47" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="5">
+        <v>33.666667938232422</v>
+      </c>
+      <c r="E47" s="6">
+        <v>0.14880295097827911</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.22165922820568085</v>
+      </c>
+      <c r="G47" s="7">
+        <v>50.600833892822266</v>
+      </c>
+      <c r="H47" s="8">
+        <v>16.934165954589844</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0</v>
+      </c>
+      <c r="J47" s="4">
+        <v>33.466178894042969</v>
+      </c>
+      <c r="K47" s="4">
+        <v>0.21764804422855377</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="5">
+        <v>0</v>
+      </c>
+      <c r="E48" s="6">
+        <v>0</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0.22165922820568085</v>
+      </c>
+      <c r="G48" s="7">
+        <v>0.2208847850561142</v>
+      </c>
+      <c r="H48" s="8">
+        <v>0.2208847850561142</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0</v>
+      </c>
+      <c r="J48" s="4">
+        <v>100</v>
+      </c>
+      <c r="K48" s="4">
+        <v>0.21764804422855377</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="5">
+        <v>28.600000381469727</v>
+      </c>
+      <c r="E49" s="6">
+        <v>3.1587202101945877E-2</v>
+      </c>
+      <c r="F49" s="4">
+        <v>3.3365894109010696E-2</v>
+      </c>
+      <c r="G49" s="7">
+        <v>30.215871810913086</v>
+      </c>
+      <c r="H49" s="8">
+        <v>1.6158726215362549</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0</v>
+      </c>
+      <c r="J49" s="4">
+        <v>5.3477606773376465</v>
+      </c>
+      <c r="K49" s="4">
+        <v>1.5336007811129093E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="5">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="E50" s="6">
+        <v>7.8003122471272945E-3</v>
+      </c>
+      <c r="F50" s="4">
+        <v>3.3365894109010696E-2</v>
+      </c>
+      <c r="G50" s="7">
+        <v>0.42884796857833862</v>
+      </c>
+      <c r="H50" s="8">
+        <v>0.3288479745388031</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0</v>
+      </c>
+      <c r="J50" s="4">
+        <v>76.681716918945312</v>
+      </c>
+      <c r="K50" s="4">
+        <v>1.5336007811129093E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1.2000000476837158</v>
+      </c>
+      <c r="E51" s="9">
+        <v>5.5376093834638596E-2</v>
+      </c>
+      <c r="F51" s="4">
+        <v>3.3365894109010696E-2</v>
+      </c>
+      <c r="G51" s="10">
+        <v>0.72144228219985962</v>
+      </c>
+      <c r="H51" s="11">
+        <v>0.4785577654838562</v>
+      </c>
+      <c r="I51" s="4">
+        <v>39.879814147949219</v>
+      </c>
+      <c r="J51" s="4">
+        <v>0</v>
+      </c>
+      <c r="K51" s="4">
+        <v>1.5335998497903347E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="5">
+        <v>8.6999998092651367</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4.0247965604066849E-2</v>
+      </c>
+      <c r="F52" s="4">
+        <v>3.3365894109010696E-2</v>
+      </c>
+      <c r="G52" s="10">
+        <v>7.2073907852172852</v>
+      </c>
+      <c r="H52" s="11">
+        <v>1.4926087856292725</v>
+      </c>
+      <c r="I52" s="4">
+        <v>17.156423568725586</v>
+      </c>
+      <c r="J52" s="4">
+        <v>0</v>
+      </c>
+      <c r="K52" s="4">
+        <v>1.5335998497903347E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0</v>
+      </c>
+      <c r="E53" s="6">
+        <v>0</v>
+      </c>
+      <c r="F53" s="4">
+        <v>3.3365894109010696E-2</v>
+      </c>
+      <c r="G53" s="7">
+        <v>2.6447299867868423E-2</v>
+      </c>
+      <c r="H53" s="8">
+        <v>2.6447299867868423E-2</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0</v>
+      </c>
+      <c r="J53" s="4">
+        <v>100</v>
+      </c>
+      <c r="K53" s="4">
+        <v>1.5336007811129093E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" s="5">
+        <v>141</v>
+      </c>
+      <c r="E54" s="6">
+        <v>0.15879987180233002</v>
+      </c>
+      <c r="F54" s="4">
+        <v>0.18595309555530548</v>
+      </c>
+      <c r="G54" s="7">
+        <v>165.33589172363281</v>
+      </c>
+      <c r="H54" s="8">
+        <v>24.335886001586914</v>
+      </c>
+      <c r="I54" s="4">
+        <v>0</v>
+      </c>
+      <c r="J54" s="4">
+        <v>14.719058036804199</v>
+      </c>
+      <c r="K54" s="4">
+        <v>0.11170246452093124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="5">
+        <v>0</v>
+      </c>
+      <c r="E55" s="6">
+        <v>0</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0.18595309555530548</v>
+      </c>
+      <c r="G55" s="7">
+        <v>2.8323664665222168</v>
+      </c>
+      <c r="H55" s="8">
+        <v>2.8323664665222168</v>
+      </c>
+      <c r="I55" s="4">
+        <v>0</v>
+      </c>
+      <c r="J55" s="4">
+        <v>100</v>
+      </c>
+      <c r="K55" s="4">
+        <v>0.11170246452093124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="5">
+        <v>0.40000000596046448</v>
+      </c>
+      <c r="E56" s="6">
+        <v>4.2507968842983246E-2</v>
+      </c>
+      <c r="F56" s="4">
+        <v>0.18595309555530548</v>
+      </c>
+      <c r="G56" s="7">
+        <v>1.7624865770339966</v>
+      </c>
+      <c r="H56" s="8">
+        <v>1.3624866008758545</v>
+      </c>
+      <c r="I56" s="4">
+        <v>0</v>
+      </c>
+      <c r="J56" s="4">
+        <v>77.304794311523438</v>
+      </c>
+      <c r="K56" s="4">
+        <v>0.11170246452093124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="5">
+        <v>73.400001525878906</v>
+      </c>
+      <c r="E57" s="9">
+        <v>0.303631991147995</v>
+      </c>
+      <c r="F57" s="4">
+        <v>0.18595309555530548</v>
+      </c>
+      <c r="G57" s="10">
+        <v>44.685325622558594</v>
+      </c>
+      <c r="H57" s="11">
+        <v>28.714675903320312</v>
+      </c>
+      <c r="I57" s="4">
+        <v>39.120811462402344</v>
+      </c>
+      <c r="J57" s="4">
+        <v>0</v>
+      </c>
+      <c r="K57" s="4">
+        <v>0.11170244216918945</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="5">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0.18595309555530548</v>
+      </c>
+      <c r="G58" s="7">
+        <v>5.255550891160965E-2</v>
+      </c>
+      <c r="H58" s="8">
+        <v>5.255550891160965E-2</v>
+      </c>
+      <c r="I58" s="4">
+        <v>0</v>
+      </c>
+      <c r="J58" s="4">
+        <v>100</v>
+      </c>
+      <c r="K58" s="4">
+        <v>0.11170246452093124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="5">
+        <v>0</v>
+      </c>
+      <c r="E59" s="6">
+        <v>0</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0.18595309555530548</v>
+      </c>
+      <c r="G59" s="7">
+        <v>0.13138876855373383</v>
+      </c>
+      <c r="H59" s="8">
+        <v>0.13138876855373383</v>
+      </c>
+      <c r="I59" s="4">
+        <v>0</v>
+      </c>
+      <c r="J59" s="4">
+        <v>100</v>
+      </c>
+      <c r="K59" s="4">
+        <v>0.11170246452093124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="5">
+        <v>2519.666748046875</v>
+      </c>
+      <c r="E60" s="6">
+        <v>0.43940189480781555</v>
+      </c>
+      <c r="F60" s="4">
+        <v>0.64173471927642822</v>
+      </c>
+      <c r="G60" s="7">
+        <v>3776.708251953125</v>
+      </c>
+      <c r="H60" s="8">
+        <v>1257.0416259765625</v>
+      </c>
+      <c r="I60" s="4">
+        <v>0</v>
+      </c>
+      <c r="J60" s="4">
+        <v>33.284053802490234</v>
+      </c>
+      <c r="K60" s="4">
+        <v>1.3537958860397339</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="5">
+        <v>221.41667175292969</v>
+      </c>
+      <c r="E61" s="9">
+        <v>1.5890388488769531</v>
+      </c>
+      <c r="F61" s="4">
+        <v>0.64173471927642822</v>
+      </c>
+      <c r="G61" s="10">
+        <v>78.406356811523438</v>
+      </c>
+      <c r="H61" s="11">
+        <v>143.01031494140625</v>
+      </c>
+      <c r="I61" s="4">
+        <v>64.588775634765625</v>
+      </c>
+      <c r="J61" s="4">
+        <v>0</v>
+      </c>
+      <c r="K61" s="4">
+        <v>1.3537960052490234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="5">
+        <v>127.75</v>
+      </c>
+      <c r="E62" s="9">
+        <v>1.0901100635528564</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0.64173471927642822</v>
+      </c>
+      <c r="G62" s="10">
+        <v>70.820884704589844</v>
+      </c>
+      <c r="H62" s="11">
+        <v>56.929111480712891</v>
+      </c>
+      <c r="I62" s="4">
+        <v>44.562904357910156</v>
+      </c>
+      <c r="J62" s="4">
+        <v>0</v>
+      </c>
+      <c r="K62" s="4">
+        <v>1.3537960052490234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="5">
         <v>1946.3333740234375</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E63" s="9">
         <v>1.2870616912841797</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F63" s="4">
         <v>0.64173471927642822</v>
       </c>
-      <c r="G47" s="10">
+      <c r="G63" s="10">
         <v>889.02947998046875</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H63" s="11">
         <v>1057.3038330078125</v>
       </c>
-      <c r="I47" s="4">
+      <c r="I63" s="4">
         <v>54.322856903076172</v>
       </c>
-      <c r="J47" s="4">
-        <v>0</v>
-      </c>
-      <c r="K47" s="4">
+      <c r="J63" s="4">
+        <v>0</v>
+      </c>
+      <c r="K63" s="4">
         <v>1.3537960052490234</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D64" s="5">
         <v>2897.800048828125</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E64" s="9">
         <v>0.49287089705467224</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F64" s="4">
         <v>0.46806159615516663</v>
       </c>
-      <c r="G48" s="10">
+      <c r="G64" s="10">
         <v>2744.77294921875</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H64" s="11">
         <v>153.02716064453125</v>
       </c>
-      <c r="I48" s="4">
+      <c r="I64" s="4">
         <v>5.2808046340942383</v>
       </c>
-      <c r="J48" s="4">
-        <v>0</v>
-      </c>
-      <c r="K48" s="4">
+      <c r="J64" s="4">
+        <v>0</v>
+      </c>
+      <c r="K64" s="4">
         <v>0.16743750870227814</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D65" s="5">
         <v>76.5</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E65" s="9">
         <v>0.80458563566207886</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F65" s="4">
         <v>0.46806159615516663</v>
       </c>
-      <c r="G49" s="10">
+      <c r="G65" s="10">
         <v>42.932109832763672</v>
       </c>
-      <c r="H49" s="11">
+      <c r="H65" s="11">
         <v>33.567890167236328</v>
       </c>
-      <c r="I49" s="4">
+      <c r="I65" s="4">
         <v>43.879592895507812</v>
       </c>
-      <c r="J49" s="4">
-        <v>0</v>
-      </c>
-      <c r="K49" s="4">
+      <c r="J65" s="4">
+        <v>0</v>
+      </c>
+      <c r="K65" s="4">
         <v>0.16743750870227814</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D66" s="5">
         <v>27.899999618530273</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E66" s="6">
         <v>0.38621264696121216</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F66" s="4">
         <v>0.46806159615516663</v>
       </c>
-      <c r="G50" s="7">
+      <c r="G66" s="7">
         <v>34.103111267089844</v>
       </c>
-      <c r="H50" s="8">
+      <c r="H66" s="8">
         <v>6.2031121253967285</v>
       </c>
-      <c r="I50" s="4">
-        <v>0</v>
-      </c>
-      <c r="J50" s="4">
+      <c r="I66" s="4">
+        <v>0</v>
+      </c>
+      <c r="J66" s="4">
         <v>18.189285278320312</v>
       </c>
-      <c r="K50" s="4">
+      <c r="K66" s="4">
         <v>0.16743765771389008</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D67" s="5">
         <v>503.60000610351562</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E67" s="6">
         <v>0.34892743825912476</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F67" s="4">
         <v>0.46806159615516663</v>
       </c>
-      <c r="G51" s="7">
+      <c r="G67" s="7">
         <v>683.9871826171875</v>
       </c>
-      <c r="H51" s="8">
+      <c r="H67" s="8">
         <v>180.38717651367188</v>
       </c>
-      <c r="I51" s="4">
-        <v>0</v>
-      </c>
-      <c r="J51" s="4">
+      <c r="I67" s="4">
+        <v>0</v>
+      </c>
+      <c r="J67" s="4">
         <v>26.372888565063477</v>
       </c>
-      <c r="K51" s="4">
+      <c r="K67" s="4">
         <v>0.16743765771389008</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D68" s="5">
         <v>1876.800048828125</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E68" s="6">
         <v>0.36263161897659302</v>
       </c>
-      <c r="F52" s="4">
+      <c r="F68" s="4">
         <v>0.78190147876739502</v>
       </c>
-      <c r="G52" s="7">
+      <c r="G68" s="7">
         <v>4135.01611328125</v>
       </c>
-      <c r="H52" s="8">
+      <c r="H68" s="8">
         <v>2258.21630859375</v>
       </c>
-      <c r="I52" s="4">
-        <v>0</v>
-      </c>
-      <c r="J52" s="4">
+      <c r="I68" s="4">
+        <v>0</v>
+      </c>
+      <c r="J68" s="4">
         <v>54.612026214599609</v>
       </c>
-      <c r="K52" s="4">
+      <c r="K68" s="4">
         <v>1.0131837129592896</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B69" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D69" s="5">
         <v>119.19999694824219</v>
       </c>
-      <c r="E53" s="9">
+      <c r="E69" s="9">
         <v>1.0723282098770142</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F69" s="4">
         <v>0.78190147876739502</v>
       </c>
-      <c r="G53" s="10">
+      <c r="G69" s="10">
         <v>85.602668762207031</v>
       </c>
-      <c r="H53" s="11">
+      <c r="H69" s="11">
         <v>33.597328186035156</v>
       </c>
-      <c r="I53" s="4">
+      <c r="I69" s="4">
         <v>28.185676574707031</v>
       </c>
-      <c r="J53" s="4">
-        <v>0</v>
-      </c>
-      <c r="K53" s="4">
+      <c r="J69" s="4">
+        <v>0</v>
+      </c>
+      <c r="K69" s="4">
         <v>1.0131838321685791</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D70" s="5">
         <v>67.199996948242188</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E70" s="9">
         <v>1.1315035820007324</v>
       </c>
-      <c r="F54" s="4">
+      <c r="F70" s="4">
         <v>0.78190147876739502</v>
       </c>
-      <c r="G54" s="10">
+      <c r="G70" s="10">
         <v>45.592376708984375</v>
       </c>
-      <c r="H54" s="11">
+      <c r="H70" s="11">
         <v>21.607620239257812</v>
       </c>
-      <c r="I54" s="4">
+      <c r="I70" s="4">
         <v>32.154197692871094</v>
       </c>
-      <c r="J54" s="4">
-        <v>0</v>
-      </c>
-      <c r="K54" s="4">
+      <c r="J70" s="4">
+        <v>0</v>
+      </c>
+      <c r="K70" s="4">
         <v>1.0131838321685791</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D71" s="5">
         <v>3603</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E71" s="9">
         <v>1.895308256149292</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F71" s="4">
         <v>0.78190147876739502</v>
       </c>
-      <c r="G55" s="10">
+      <c r="G71" s="10">
         <v>1400.287353515625</v>
       </c>
-      <c r="H55" s="11">
+      <c r="H71" s="11">
         <v>2202.712646484375</v>
       </c>
-      <c r="I55" s="4">
+      <c r="I71" s="4">
         <v>61.135517120361328</v>
       </c>
-      <c r="J55" s="4">
-        <v>0</v>
-      </c>
-      <c r="K55" s="4">
+      <c r="J71" s="4">
+        <v>0</v>
+      </c>
+      <c r="K71" s="4">
         <v>1.0131838321685791</v>
       </c>
     </row>
@@ -6403,9 +8089,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEACAC12-7817-3D46-BCD9-D2A9C41AD50E}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7932,419 +9618,979 @@
       <c r="A44" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>27</v>
+      <c r="B44" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D44" s="10">
-        <v>1765.5</v>
-      </c>
-      <c r="E44" s="9">
-        <v>0.3010522723197937</v>
+        <v>16.166666030883789</v>
+      </c>
+      <c r="E44" s="6">
+        <v>1.7997557297348976E-2</v>
       </c>
       <c r="F44" s="4">
-        <v>0.29376664757728577</v>
-      </c>
-      <c r="G44" s="10">
-        <v>1721.2127685546875</v>
-      </c>
-      <c r="H44" s="11">
-        <v>44.287250518798828</v>
+        <v>2.3560682311654091E-2</v>
+      </c>
+      <c r="G44" s="7">
+        <v>21.178024291992188</v>
+      </c>
+      <c r="H44" s="8">
+        <v>5.0113568305969238</v>
       </c>
       <c r="I44" s="4">
-        <v>2.5084822177886963</v>
+        <v>0</v>
       </c>
       <c r="J44" s="4">
-        <v>0</v>
+        <v>23.663003921508789</v>
       </c>
       <c r="K44" s="4">
-        <v>4.7688387334346771E-2</v>
+        <v>5.2317220717668533E-2</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>27</v>
+      <c r="B45" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="10">
-        <v>1.9166666269302368</v>
+        <v>0</v>
       </c>
       <c r="E45" s="6">
-        <v>0.1510375589132309</v>
+        <v>0</v>
       </c>
       <c r="F45" s="4">
-        <v>0.29376664757728577</v>
+        <v>2.3560682311654091E-2</v>
       </c>
       <c r="G45" s="7">
-        <v>3.794081449508667</v>
+        <v>8.7894238531589508E-2</v>
       </c>
       <c r="H45" s="8">
-        <v>1.8774147033691406</v>
+        <v>8.7894238531589508E-2</v>
       </c>
       <c r="I45" s="4">
         <v>0</v>
       </c>
       <c r="J45" s="4">
-        <v>49.482719421386719</v>
+        <v>100</v>
       </c>
       <c r="K45" s="4">
-        <v>4.7688327729701996E-2</v>
+        <v>5.2317220717668533E-2</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>27</v>
+      <c r="B46" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D46" s="10">
-        <v>15.25</v>
+        <v>0</v>
       </c>
       <c r="E46" s="6">
-        <v>0.20745475590229034</v>
+        <v>0</v>
       </c>
       <c r="F46" s="4">
-        <v>0.29376664757728577</v>
+        <v>2.3560682311654091E-2</v>
       </c>
       <c r="G46" s="7">
-        <v>21.826625823974609</v>
+        <v>0.45033982396125793</v>
       </c>
       <c r="H46" s="8">
-        <v>6.5766263008117676</v>
+        <v>0.45033982396125793</v>
       </c>
       <c r="I46" s="4">
         <v>0</v>
       </c>
       <c r="J46" s="4">
-        <v>30.131208419799805</v>
+        <v>100</v>
       </c>
       <c r="K46" s="4">
-        <v>4.7688327729701996E-2</v>
+        <v>5.2317220717668533E-2</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>27</v>
+      <c r="B47" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="10">
-        <v>325.75</v>
-      </c>
-      <c r="E47" s="6">
-        <v>0.26607909798622131</v>
+        <v>10.583333015441895</v>
+      </c>
+      <c r="E47" s="9">
+        <v>4.860537126660347E-2</v>
       </c>
       <c r="F47" s="4">
-        <v>0.29376664757728577</v>
-      </c>
-      <c r="G47" s="7">
-        <v>360.88534545898438</v>
-      </c>
-      <c r="H47" s="8">
-        <v>35.135349273681641</v>
+        <v>2.3560682311654091E-2</v>
+      </c>
+      <c r="G47" s="10">
+        <v>5.1146407127380371</v>
+      </c>
+      <c r="H47" s="11">
+        <v>5.4686923027038574</v>
       </c>
       <c r="I47" s="4">
-        <v>0</v>
+        <v>51.672679901123047</v>
       </c>
       <c r="J47" s="4">
-        <v>9.7358760833740234</v>
+        <v>0</v>
       </c>
       <c r="K47" s="4">
-        <v>4.7688327729701996E-2</v>
+        <v>5.2317224442958832E-2</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D48" s="10">
-        <v>2002.5999755859375</v>
-      </c>
-      <c r="E48" s="6">
-        <v>0.34923118352890015</v>
+        <v>0.1666666716337204</v>
+      </c>
+      <c r="E48" s="9">
+        <v>0.12254901975393295</v>
       </c>
       <c r="F48" s="4">
-        <v>0.48498272895812988</v>
-      </c>
-      <c r="G48" s="7">
-        <v>2820.71875</v>
-      </c>
-      <c r="H48" s="8">
-        <v>818.1187744140625</v>
+        <v>2.3560682311654091E-2</v>
+      </c>
+      <c r="G48" s="10">
+        <v>3.1660828739404678E-2</v>
+      </c>
+      <c r="H48" s="11">
+        <v>0.13500584661960602</v>
       </c>
       <c r="I48" s="4">
-        <v>0</v>
+        <v>81.003501892089844</v>
       </c>
       <c r="J48" s="4">
-        <v>29.003911972045898</v>
+        <v>0</v>
       </c>
       <c r="K48" s="4">
-        <v>0.73425143957138062</v>
+        <v>5.2317224442958832E-2</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D49" s="10">
-        <v>160.30000305175781</v>
-      </c>
-      <c r="E49" s="9">
-        <v>1.1504234075546265</v>
+        <v>0</v>
+      </c>
+      <c r="E49" s="6">
+        <v>0</v>
       </c>
       <c r="F49" s="4">
-        <v>0.48498272895812988</v>
-      </c>
-      <c r="G49" s="10">
-        <v>62.851413726806641</v>
-      </c>
-      <c r="H49" s="11">
-        <v>97.448593139648438</v>
+        <v>2.3560682311654091E-2</v>
+      </c>
+      <c r="G49" s="7">
+        <v>5.4106935858726501E-2</v>
+      </c>
+      <c r="H49" s="8">
+        <v>5.4106935858726501E-2</v>
       </c>
       <c r="I49" s="4">
-        <v>60.791385650634766</v>
+        <v>0</v>
       </c>
       <c r="J49" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K49" s="4">
-        <v>0.73425126075744629</v>
+        <v>5.2317220717668533E-2</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>27</v>
+      <c r="B50" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D50" s="10">
-        <v>170.5</v>
+        <v>146.89999389648438</v>
       </c>
       <c r="E50" s="9">
-        <v>1.4549022912979126</v>
+        <v>0.1618179976940155</v>
       </c>
       <c r="F50" s="4">
-        <v>0.48498272895812988</v>
+        <v>0.1480766236782074</v>
       </c>
       <c r="G50" s="10">
-        <v>51.041603088378906</v>
+        <v>134.23794555664062</v>
       </c>
       <c r="H50" s="11">
-        <v>119.45839691162109</v>
+        <v>12.662052154541016</v>
       </c>
       <c r="I50" s="4">
-        <v>70.063575744628906</v>
+        <v>8.6195049285888672</v>
       </c>
       <c r="J50" s="4">
         <v>0</v>
       </c>
       <c r="K50" s="4">
-        <v>0.73425126075744629</v>
+        <v>9.8512835800647736E-2</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>27</v>
+      <c r="B51" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D51" s="10">
-        <v>1305.5</v>
-      </c>
-      <c r="E51" s="9">
-        <v>0.86329460144042969</v>
+        <v>0.60000002384185791</v>
+      </c>
+      <c r="E51" s="6">
+        <v>2.5178346782922745E-2</v>
       </c>
       <c r="F51" s="4">
-        <v>0.48498272895812988</v>
-      </c>
-      <c r="G51" s="10">
-        <v>704.24566650390625</v>
-      </c>
-      <c r="H51" s="11">
-        <v>601.25433349609375</v>
+        <v>0.1480766236782074</v>
+      </c>
+      <c r="G51" s="7">
+        <v>3.5726845264434814</v>
+      </c>
+      <c r="H51" s="8">
+        <v>2.972684383392334</v>
       </c>
       <c r="I51" s="4">
-        <v>46.055484771728516</v>
+        <v>0</v>
       </c>
       <c r="J51" s="4">
-        <v>0</v>
+        <v>83.205902099609375</v>
       </c>
       <c r="K51" s="4">
-        <v>0.73425126075744629</v>
+        <v>9.8512835800647736E-2</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D52" s="10">
-        <v>8712.7998046875</v>
-      </c>
-      <c r="E52" s="9">
-        <v>1.48191237449646</v>
+        <v>0</v>
+      </c>
+      <c r="E52" s="6">
+        <v>0</v>
       </c>
       <c r="F52" s="4">
-        <v>1.4043182134628296</v>
-      </c>
-      <c r="G52" s="10">
-        <v>8222.1376953125</v>
-      </c>
-      <c r="H52" s="11">
-        <v>490.66171264648438</v>
+        <v>0.1480766236782074</v>
+      </c>
+      <c r="G52" s="7">
+        <v>1.7254698276519775</v>
+      </c>
+      <c r="H52" s="8">
+        <v>1.7254698276519775</v>
       </c>
       <c r="I52" s="4">
-        <v>5.6315045356750488</v>
+        <v>0</v>
       </c>
       <c r="J52" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K52" s="4">
-        <v>0.43672475218772888</v>
+        <v>9.8512835800647736E-2</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D53" s="10">
-        <v>490.20001220703125</v>
-      </c>
-      <c r="E53" s="9">
-        <v>5.1556582450866699</v>
+        <v>25.799999237060547</v>
+      </c>
+      <c r="E53" s="6">
+        <v>0.11403314769268036</v>
       </c>
       <c r="F53" s="4">
-        <v>1.4043182134628296</v>
-      </c>
-      <c r="G53" s="10">
-        <v>106.58685302734375</v>
-      </c>
-      <c r="H53" s="11">
-        <v>383.6131591796875</v>
+        <v>0.1480766236782074</v>
+      </c>
+      <c r="G53" s="7">
+        <v>33.61810302734375</v>
+      </c>
+      <c r="H53" s="8">
+        <v>7.8181047439575195</v>
       </c>
       <c r="I53" s="4">
-        <v>78.256462097167969</v>
+        <v>0</v>
       </c>
       <c r="J53" s="4">
-        <v>0</v>
+        <v>23.255638122558594</v>
       </c>
       <c r="K53" s="4">
-        <v>0.43672475218772888</v>
+        <v>9.8512835800647736E-2</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D54" s="10">
-        <v>193.60000610351562</v>
-      </c>
-      <c r="E54" s="9">
-        <v>2.6799557209014893</v>
+        <v>0</v>
+      </c>
+      <c r="E54" s="6">
+        <v>0</v>
       </c>
       <c r="F54" s="4">
-        <v>1.4043182134628296</v>
-      </c>
-      <c r="G54" s="10">
-        <v>94.48876953125</v>
-      </c>
-      <c r="H54" s="11">
-        <v>99.111236572265625</v>
+        <v>0.1480766236782074</v>
+      </c>
+      <c r="G54" s="7">
+        <v>0.14579316973686218</v>
+      </c>
+      <c r="H54" s="8">
+        <v>0.14579316973686218</v>
       </c>
       <c r="I54" s="4">
-        <v>51.193820953369141</v>
+        <v>0</v>
       </c>
       <c r="J54" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K54" s="4">
-        <v>0.43672475218772888</v>
+        <v>9.8512835800647736E-2</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="10">
+        <v>227.60000610351562</v>
+      </c>
+      <c r="E55" s="9">
+        <v>0.25137227773666382</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0.21575458347797394</v>
+      </c>
+      <c r="G55" s="10">
+        <v>194.99899291992188</v>
+      </c>
+      <c r="H55" s="11">
+        <v>32.601020812988281</v>
+      </c>
+      <c r="I55" s="4">
+        <v>14.323822021484375</v>
+      </c>
+      <c r="J55" s="4">
+        <v>0</v>
+      </c>
+      <c r="K55" s="4">
+        <v>0.1268206387758255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="10">
+        <v>0.80000001192092896</v>
+      </c>
+      <c r="E56" s="6">
+        <v>6.2402497977018356E-2</v>
+      </c>
+      <c r="F56" s="4">
+        <v>0.21575458347797394</v>
+      </c>
+      <c r="G56" s="7">
+        <v>2.7874133586883545</v>
+      </c>
+      <c r="H56" s="8">
+        <v>1.9874134063720703</v>
+      </c>
+      <c r="I56" s="4">
+        <v>0</v>
+      </c>
+      <c r="J56" s="4">
+        <v>71.299560546875</v>
+      </c>
+      <c r="K56" s="4">
+        <v>0.12682065367698669</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="10">
+        <v>2.5999999046325684</v>
+      </c>
+      <c r="E57" s="6">
+        <v>0.1199815422296524</v>
+      </c>
+      <c r="F57" s="4">
+        <v>0.21575458347797394</v>
+      </c>
+      <c r="G57" s="7">
+        <v>4.6980347633361816</v>
+      </c>
+      <c r="H57" s="8">
+        <v>2.0980348587036133</v>
+      </c>
+      <c r="I57" s="4">
+        <v>0</v>
+      </c>
+      <c r="J57" s="4">
+        <v>44.657711029052734</v>
+      </c>
+      <c r="K57" s="4">
+        <v>0.12682065367698669</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="10">
+        <v>18.600000381469727</v>
+      </c>
+      <c r="E58" s="6">
+        <v>8.6047373712062836E-2</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0.21575458347797394</v>
+      </c>
+      <c r="G58" s="7">
+        <v>46.943271636962891</v>
+      </c>
+      <c r="H58" s="8">
+        <v>28.343271255493164</v>
+      </c>
+      <c r="I58" s="4">
+        <v>0</v>
+      </c>
+      <c r="J58" s="4">
+        <v>60.377708435058594</v>
+      </c>
+      <c r="K58" s="4">
+        <v>0.12682065367698669</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="10">
+        <v>0</v>
+      </c>
+      <c r="E59" s="6">
+        <v>0</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0.21575458347797394</v>
+      </c>
+      <c r="G59" s="7">
+        <v>0.1723048985004425</v>
+      </c>
+      <c r="H59" s="8">
+        <v>0.1723048985004425</v>
+      </c>
+      <c r="I59" s="4">
+        <v>0</v>
+      </c>
+      <c r="J59" s="4">
+        <v>100</v>
+      </c>
+      <c r="K59" s="4">
+        <v>0.12682065367698669</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C60" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="10">
+        <v>1765.5</v>
+      </c>
+      <c r="E60" s="9">
+        <v>0.3010522723197937</v>
+      </c>
+      <c r="F60" s="4">
+        <v>0.29376664757728577</v>
+      </c>
+      <c r="G60" s="10">
+        <v>1721.2127685546875</v>
+      </c>
+      <c r="H60" s="11">
+        <v>44.287250518798828</v>
+      </c>
+      <c r="I60" s="4">
+        <v>2.5084822177886963</v>
+      </c>
+      <c r="J60" s="4">
+        <v>0</v>
+      </c>
+      <c r="K60" s="4">
+        <v>4.7688387334346771E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="10">
+        <v>1.9166666269302368</v>
+      </c>
+      <c r="E61" s="6">
+        <v>0.1510375589132309</v>
+      </c>
+      <c r="F61" s="4">
+        <v>0.29376664757728577</v>
+      </c>
+      <c r="G61" s="7">
+        <v>3.794081449508667</v>
+      </c>
+      <c r="H61" s="8">
+        <v>1.8774147033691406</v>
+      </c>
+      <c r="I61" s="4">
+        <v>0</v>
+      </c>
+      <c r="J61" s="4">
+        <v>49.482719421386719</v>
+      </c>
+      <c r="K61" s="4">
+        <v>4.7688327729701996E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="10">
+        <v>15.25</v>
+      </c>
+      <c r="E62" s="6">
+        <v>0.20745475590229034</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0.29376664757728577</v>
+      </c>
+      <c r="G62" s="7">
+        <v>21.826625823974609</v>
+      </c>
+      <c r="H62" s="8">
+        <v>6.5766263008117676</v>
+      </c>
+      <c r="I62" s="4">
+        <v>0</v>
+      </c>
+      <c r="J62" s="4">
+        <v>30.131208419799805</v>
+      </c>
+      <c r="K62" s="4">
+        <v>4.7688327729701996E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D63" s="10">
+        <v>325.75</v>
+      </c>
+      <c r="E63" s="6">
+        <v>0.26607909798622131</v>
+      </c>
+      <c r="F63" s="4">
+        <v>0.29376664757728577</v>
+      </c>
+      <c r="G63" s="7">
+        <v>360.88534545898438</v>
+      </c>
+      <c r="H63" s="8">
+        <v>35.135349273681641</v>
+      </c>
+      <c r="I63" s="4">
+        <v>0</v>
+      </c>
+      <c r="J63" s="4">
+        <v>9.7358760833740234</v>
+      </c>
+      <c r="K63" s="4">
+        <v>4.7688327729701996E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" s="10">
+        <v>2002.5999755859375</v>
+      </c>
+      <c r="E64" s="6">
+        <v>0.34923118352890015</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0.48498272895812988</v>
+      </c>
+      <c r="G64" s="7">
+        <v>2820.71875</v>
+      </c>
+      <c r="H64" s="8">
+        <v>818.1187744140625</v>
+      </c>
+      <c r="I64" s="4">
+        <v>0</v>
+      </c>
+      <c r="J64" s="4">
+        <v>29.003911972045898</v>
+      </c>
+      <c r="K64" s="4">
+        <v>0.73425143957138062</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="10">
+        <v>160.30000305175781</v>
+      </c>
+      <c r="E65" s="9">
+        <v>1.1504234075546265</v>
+      </c>
+      <c r="F65" s="4">
+        <v>0.48498272895812988</v>
+      </c>
+      <c r="G65" s="10">
+        <v>62.851413726806641</v>
+      </c>
+      <c r="H65" s="11">
+        <v>97.448593139648438</v>
+      </c>
+      <c r="I65" s="4">
+        <v>60.791385650634766</v>
+      </c>
+      <c r="J65" s="4">
+        <v>0</v>
+      </c>
+      <c r="K65" s="4">
+        <v>0.73425126075744629</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" s="10">
+        <v>170.5</v>
+      </c>
+      <c r="E66" s="9">
+        <v>1.4549022912979126</v>
+      </c>
+      <c r="F66" s="4">
+        <v>0.48498272895812988</v>
+      </c>
+      <c r="G66" s="10">
+        <v>51.041603088378906</v>
+      </c>
+      <c r="H66" s="11">
+        <v>119.45839691162109</v>
+      </c>
+      <c r="I66" s="4">
+        <v>70.063575744628906</v>
+      </c>
+      <c r="J66" s="4">
+        <v>0</v>
+      </c>
+      <c r="K66" s="4">
+        <v>0.73425126075744629</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="10">
+        <v>1305.5</v>
+      </c>
+      <c r="E67" s="9">
+        <v>0.86329460144042969</v>
+      </c>
+      <c r="F67" s="4">
+        <v>0.48498272895812988</v>
+      </c>
+      <c r="G67" s="10">
+        <v>704.24566650390625</v>
+      </c>
+      <c r="H67" s="11">
+        <v>601.25433349609375</v>
+      </c>
+      <c r="I67" s="4">
+        <v>46.055484771728516</v>
+      </c>
+      <c r="J67" s="4">
+        <v>0</v>
+      </c>
+      <c r="K67" s="4">
+        <v>0.73425126075744629</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" s="10">
+        <v>8712.7998046875</v>
+      </c>
+      <c r="E68" s="9">
+        <v>1.48191237449646</v>
+      </c>
+      <c r="F68" s="4">
+        <v>1.4043182134628296</v>
+      </c>
+      <c r="G68" s="10">
+        <v>8222.1376953125</v>
+      </c>
+      <c r="H68" s="11">
+        <v>490.66171264648438</v>
+      </c>
+      <c r="I68" s="4">
+        <v>5.6315045356750488</v>
+      </c>
+      <c r="J68" s="4">
+        <v>0</v>
+      </c>
+      <c r="K68" s="4">
+        <v>0.43672475218772888</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="10">
+        <v>490.20001220703125</v>
+      </c>
+      <c r="E69" s="9">
+        <v>5.1556582450866699</v>
+      </c>
+      <c r="F69" s="4">
+        <v>1.4043182134628296</v>
+      </c>
+      <c r="G69" s="10">
+        <v>106.58685302734375</v>
+      </c>
+      <c r="H69" s="11">
+        <v>383.6131591796875</v>
+      </c>
+      <c r="I69" s="4">
+        <v>78.256462097167969</v>
+      </c>
+      <c r="J69" s="4">
+        <v>0</v>
+      </c>
+      <c r="K69" s="4">
+        <v>0.43672475218772888</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" s="10">
+        <v>193.60000610351562</v>
+      </c>
+      <c r="E70" s="9">
+        <v>2.6799557209014893</v>
+      </c>
+      <c r="F70" s="4">
+        <v>1.4043182134628296</v>
+      </c>
+      <c r="G70" s="10">
+        <v>94.48876953125</v>
+      </c>
+      <c r="H70" s="11">
+        <v>99.111236572265625</v>
+      </c>
+      <c r="I70" s="4">
+        <v>51.193820953369141</v>
+      </c>
+      <c r="J70" s="4">
+        <v>0</v>
+      </c>
+      <c r="K70" s="4">
+        <v>0.43672475218772888</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="10">
         <v>1121.800048828125</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E71" s="6">
         <v>0.77725732326507568</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F71" s="4">
         <v>1.4043182134628296</v>
       </c>
-      <c r="G55" s="7">
+      <c r="G71" s="7">
         <v>2095.17041015625</v>
       </c>
-      <c r="H55" s="8">
+      <c r="H71" s="8">
         <v>973.3704833984375</v>
       </c>
-      <c r="I55" s="4">
-        <v>0</v>
-      </c>
-      <c r="J55" s="4">
+      <c r="I71" s="4">
+        <v>0</v>
+      </c>
+      <c r="J71" s="4">
         <v>46.457817077636719</v>
       </c>
-      <c r="K55" s="4">
+      <c r="K71" s="4">
         <v>0.43672454357147217</v>
       </c>
     </row>

</xml_diff>